<commit_message>
changed results graphs in persentation
</commit_message>
<xml_diff>
--- a/summary_table.xlsx
+++ b/summary_table.xlsx
@@ -248,19 +248,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.41322314049587133</c:v>
+                  <c:v>-0.41322314049587133</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6018371872030337</c:v>
+                  <c:v>-0.6018371872030337</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1808576755748947</c:v>
+                  <c:v>-1.1808576755748947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5534572037770402</c:v>
+                  <c:v>-1.5534572037770402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4165159734779953</c:v>
+                  <c:v>-1.4165159734779953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -326,19 +326,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.4011443102352339</c:v>
+                  <c:v>-3.4011443102352339</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3123218245169501</c:v>
+                  <c:v>-2.3123218245169501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5425730267246847</c:v>
+                  <c:v>-3.5425730267246847</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8684130368565302</c:v>
+                  <c:v>-3.8684130368565302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.737191078963241</c:v>
+                  <c:v>-3.737191078963241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,7 +427,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -465,7 +465,7 @@
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="0"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -473,6 +473,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
+          <c:min val="-4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -524,7 +525,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percent</a:t>
+                  <a:t>Percent Change</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -947,7 +948,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -993,6 +994,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
+          <c:min val="-4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1044,7 +1046,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percent</a:t>
+                  <a:t>Percent Change</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1089,7 +1091,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1906,19 +1908,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.19531250000000278</c:v>
+                  <c:v>-0.19531250000000278</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68493150684931781</c:v>
+                  <c:v>-0.68493150684931781</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1700288184438015</c:v>
+                  <c:v>-3.1700288184438015</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4883720930232642</c:v>
+                  <c:v>-3.4883720930232642</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9980657640232189</c:v>
+                  <c:v>-2.9980657640232189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,19 +1986,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.0312500000000027</c:v>
+                  <c:v>-7.0312500000000027</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3052837573385574</c:v>
+                  <c:v>-4.3052837573385574</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9731027857828982</c:v>
+                  <c:v>-7.9731027857828982</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.2364341085271313</c:v>
+                  <c:v>-8.2364341085271313</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5435203094777661</c:v>
+                  <c:v>-7.5435203094777661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2085,7 +2087,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2183,6 +2185,11 @@
                   <a:rPr lang="en-US"/>
                   <a:t>Percent</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Change</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4625,16 +4632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>311727</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>422275</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>11257</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4963,8 +4970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5052,12 +5059,12 @@
         <v>0.5</v>
       </c>
       <c r="P3">
-        <f>D5</f>
-        <v>0.41322314049587133</v>
+        <f>-D5</f>
+        <v>-0.41322314049587133</v>
       </c>
       <c r="Q3">
-        <f>D6</f>
-        <v>3.4011443102352339</v>
+        <f>-D6</f>
+        <v>-3.4011443102352339</v>
       </c>
       <c r="S3">
         <v>50</v>
@@ -5109,12 +5116,12 @@
         <v>0.6</v>
       </c>
       <c r="P4">
-        <f>D9</f>
-        <v>0.6018371872030337</v>
+        <f>-D9</f>
+        <v>-0.6018371872030337</v>
       </c>
       <c r="Q4">
-        <f>D10</f>
-        <v>2.3123218245169501</v>
+        <f>-D10</f>
+        <v>-2.3123218245169501</v>
       </c>
       <c r="S4">
         <v>60</v>
@@ -5182,12 +5189,12 @@
         <v>0.7</v>
       </c>
       <c r="P5">
-        <f>D13</f>
-        <v>1.1808576755748947</v>
+        <f>-D13</f>
+        <v>-1.1808576755748947</v>
       </c>
       <c r="Q5">
-        <f>D14</f>
-        <v>3.5425730267246847</v>
+        <f>-D14</f>
+        <v>-3.5425730267246847</v>
       </c>
       <c r="S5">
         <v>70</v>
@@ -5255,12 +5262,12 @@
         <v>0.8</v>
       </c>
       <c r="P6">
-        <f>D17</f>
-        <v>1.5534572037770402</v>
+        <f>-D17</f>
+        <v>-1.5534572037770402</v>
       </c>
       <c r="Q6">
-        <f>D18</f>
-        <v>3.8684130368565302</v>
+        <f>-D18</f>
+        <v>-3.8684130368565302</v>
       </c>
       <c r="S6">
         <v>80</v>
@@ -5297,12 +5304,12 @@
         <v>0.9</v>
       </c>
       <c r="P7">
-        <f>D21</f>
-        <v>1.4165159734779953</v>
+        <f>-D21</f>
+        <v>-1.4165159734779953</v>
       </c>
       <c r="Q7">
-        <f>D22</f>
-        <v>3.737191078963241</v>
+        <f>-D22</f>
+        <v>-3.737191078963241</v>
       </c>
       <c r="S7">
         <v>90</v>
@@ -6037,12 +6044,12 @@
         <v>0.5</v>
       </c>
       <c r="C26">
-        <f>F5</f>
-        <v>0.19531250000000278</v>
+        <f>-F5</f>
+        <v>-0.19531250000000278</v>
       </c>
       <c r="D26">
-        <f>F6</f>
-        <v>7.0312500000000027</v>
+        <f>-F6</f>
+        <v>-7.0312500000000027</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.35">
@@ -6050,12 +6057,12 @@
         <v>0.6</v>
       </c>
       <c r="C27">
-        <f>F9</f>
-        <v>0.68493150684931781</v>
+        <f>-F9</f>
+        <v>-0.68493150684931781</v>
       </c>
       <c r="D27">
-        <f>F10</f>
-        <v>4.3052837573385574</v>
+        <f>-F10</f>
+        <v>-4.3052837573385574</v>
       </c>
       <c r="P27" t="s">
         <v>12</v>
@@ -6069,12 +6076,12 @@
         <v>0.7</v>
       </c>
       <c r="C28">
-        <f>F13</f>
-        <v>3.1700288184438015</v>
+        <f>-F13</f>
+        <v>-3.1700288184438015</v>
       </c>
       <c r="D28">
-        <f>F14</f>
-        <v>7.9731027857828982</v>
+        <f>-F14</f>
+        <v>-7.9731027857828982</v>
       </c>
       <c r="O28" s="3">
         <v>0.5</v>
@@ -6093,12 +6100,12 @@
         <v>0.8</v>
       </c>
       <c r="C29">
-        <f>F17</f>
-        <v>3.4883720930232642</v>
+        <f>-F17</f>
+        <v>-3.4883720930232642</v>
       </c>
       <c r="D29">
-        <f>F18</f>
-        <v>8.2364341085271313</v>
+        <f>-F18</f>
+        <v>-8.2364341085271313</v>
       </c>
       <c r="O29" s="3">
         <v>0.6</v>
@@ -6117,12 +6124,12 @@
         <v>0.9</v>
       </c>
       <c r="C30">
-        <f>F21</f>
-        <v>2.9980657640232189</v>
+        <f>-F21</f>
+        <v>-2.9980657640232189</v>
       </c>
       <c r="D30">
-        <f>F22</f>
-        <v>7.5435203094777661</v>
+        <f>-F22</f>
+        <v>-7.5435203094777661</v>
       </c>
       <c r="O30" s="3">
         <v>0.7</v>

</xml_diff>